<commit_message>
chore: add generate-demos cmds to makefilecr
</commit_message>
<xml_diff>
--- a/services/worker/demos/report/output/balance/ytd/balance-ytd.xlsx
+++ b/services/worker/demos/report/output/balance/ytd/balance-ytd.xlsx
@@ -17,7 +17,7 @@
     <t>דוח מאזן - דוגמה בע"מ - Demo Business Ltd</t>
   </si>
   <si>
-    <t>תקופה: 2026-01-01 עד 2026-02-12</t>
+    <t>תקופה: 2026-01-01 עד 2026-02-13</t>
   </si>
   <si>
     <t>מדד</t>
@@ -239,7 +239,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/2026-008.pdf</t>
   </si>
   <si>
-    <t>2026-01-09</t>
+    <t>2026-01-10</t>
   </si>
   <si>
     <t>עסק ט' - מסעדה</t>
@@ -254,7 +254,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/2026-009.pdf</t>
   </si>
   <si>
-    <t>2026-01-10</t>
+    <t>2026-01-11</t>
   </si>
   <si>
     <t>לקוח י' בע"מ</t>
@@ -338,7 +338,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/2026-016.pdf</t>
   </si>
   <si>
-    <t>2026-01-18</t>
+    <t>2026-01-19</t>
   </si>
   <si>
     <t>עסק יז' - אופנה</t>
@@ -350,7 +350,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/2026-017.pdf</t>
   </si>
   <si>
-    <t>2026-01-19</t>
+    <t>2026-01-20</t>
   </si>
   <si>
     <t>לקוח יח' - נדל"ן</t>
@@ -362,7 +362,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/2026-018.pdf</t>
   </si>
   <si>
-    <t>2026-01-20</t>
+    <t>2026-01-21</t>
   </si>
   <si>
     <t>חברה יט' - פיננסים</t>
@@ -425,7 +425,7 @@
     <t>הוצאה</t>
   </si>
   <si>
-    <t>2026-01-26</t>
+    <t>2026-01-27</t>
   </si>
   <si>
     <t>Google Cloud Platform</t>
@@ -437,7 +437,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-001.pdf</t>
   </si>
   <si>
-    <t>2026-01-27</t>
+    <t>2026-01-28</t>
   </si>
   <si>
     <t>משרד רואה חשבון</t>
@@ -449,7 +449,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-002.pdf</t>
   </si>
   <si>
-    <t>2026-01-28</t>
+    <t>2026-01-29</t>
   </si>
   <si>
     <t>Office Depot</t>
@@ -461,7 +461,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-003.pdf</t>
   </si>
   <si>
-    <t>2026-01-29</t>
+    <t>2026-01-30</t>
   </si>
   <si>
     <t>חברת חשמל</t>
@@ -473,7 +473,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-004.pdf</t>
   </si>
   <si>
-    <t>2026-01-30</t>
+    <t>2026-01-31</t>
   </si>
   <si>
     <t>GitHub Enterprise</t>
@@ -488,7 +488,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-005.pdf</t>
   </si>
   <si>
-    <t>2026-01-31</t>
+    <t>2026-02-01</t>
   </si>
   <si>
     <t>משרד עורך דין</t>
@@ -524,7 +524,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-008.pdf</t>
   </si>
   <si>
-    <t>2026-02-04</t>
+    <t>2026-02-05</t>
   </si>
   <si>
     <t>Adobe Creative Cloud</t>
@@ -533,7 +533,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-009.pdf</t>
   </si>
   <si>
-    <t>2026-02-05</t>
+    <t>2026-02-06</t>
   </si>
   <si>
     <t>משלוח ארוחות</t>
@@ -545,7 +545,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-010.pdf</t>
   </si>
   <si>
-    <t>2026-02-06</t>
+    <t>2026-02-07</t>
   </si>
   <si>
     <t>AWS</t>
@@ -557,7 +557,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-011.pdf</t>
   </si>
   <si>
-    <t>2026-02-07</t>
+    <t>2026-02-08</t>
   </si>
   <si>
     <t>חניון חודשי</t>
@@ -569,7 +569,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-012.pdf</t>
   </si>
   <si>
-    <t>2026-02-08</t>
+    <t>2026-02-09</t>
   </si>
   <si>
     <t>Zoom Pro</t>
@@ -578,7 +578,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-013.pdf</t>
   </si>
   <si>
-    <t>2026-02-09</t>
+    <t>2026-02-10</t>
   </si>
   <si>
     <t>ביטוח לאומי</t>
@@ -590,7 +590,7 @@
     <t>https://storage.googleapis.com/demo-bucket-invoices/EXP-014.pdf</t>
   </si>
   <si>
-    <t>2026-02-10</t>
+    <t>2026-02-11</t>
   </si>
   <si>
     <t>ניקיון משרדים</t>
@@ -607,7 +607,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="₪#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]-#,##0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>

</xml_diff>